<commit_message>
comments + minor refactor
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+  <si>
+    <t>Points on Bench</t>
+  </si>
   <si>
     <t>3</t>
   </si>
@@ -417,60 +420,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A10"/>
+  <dimension ref="B1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:2">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="2:2">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="2:2">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="2:2">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="1" t="s">
+    <row r="5" spans="2:2">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="1" t="s">
+    <row r="6" spans="2:2">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="1" t="s">
+    <row r="7" spans="2:2">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1" t="s">
+    <row r="8" spans="2:2">
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
+      <c r="B10" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
getting data and graphs into excel
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -8,13 +8,41 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>points_vec</t>
+  </si>
+  <si>
+    <t>rank_vec</t>
+  </si>
+  <si>
+    <t>overall_rank_vec</t>
+  </si>
+  <si>
+    <t>bank_vec</t>
+  </si>
+  <si>
+    <t>team_value_vec</t>
+  </si>
+  <si>
+    <t>event_transfers_vec</t>
+  </si>
+  <si>
+    <t>event_transfer_cost_vec</t>
+  </si>
   <si>
     <t>Points on Bench</t>
   </si>
@@ -23,17 +51,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -59,9 +80,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -72,6 +92,307 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="points.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="381000"/>
+          <a:ext cx="6667500" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="gw_rank.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="381000"/>
+          <a:ext cx="6667500" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="overall_rank.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="381000"/>
+          <a:ext cx="6667500" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="bank.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="381000"/>
+          <a:ext cx="6667500" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="team_value.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="381000"/>
+          <a:ext cx="6667500" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="event_transfers.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="381000"/>
+          <a:ext cx="6667500" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="transfer_cost.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="381000"/>
+          <a:ext cx="6667500" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -406,57 +727,540 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="1">
+      <c r="A2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>2753183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>6813049</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>8375957</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>1348717</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>4456049</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>6497294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>6582907</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>4402848</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>408092</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>662945</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>2753181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>5394590</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>6241850</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>4466846</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>4132105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>4685805</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>4634337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>4503149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>2960579</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>2131984</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>5</v>
+      </c>
+    </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="1">
+      <c r="A3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
         <v>10</v>
       </c>
     </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>1003</v>
+      </c>
+    </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="1">
+      <c r="A4">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>1011</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="1">
+      <c r="A6">
         <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="1">
+      <c r="A7">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="1">
+      <c r="A8">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="1">
+      <c r="A9">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="1">
+      <c r="A10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="1">
+      <c r="A11">
         <v>7</v>
       </c>
     </row>

</xml_diff>